<commit_message>
added endpoint for batch report and its all required dropdowns , updated api-docs ready for integration"
</commit_message>
<xml_diff>
--- a/BatchReports_All.xlsx
+++ b/BatchReports_All.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="1756-1" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="1756-3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>CEAT LIMITED AMBARNATH : MIXER 1</t>
   </si>
@@ -43,13 +43,13 @@
     <t>Set Batchs</t>
   </si>
   <si>
-    <t>02:35:19</t>
+    <t>04:00:10</t>
   </si>
   <si>
     <t>MT671</t>
   </si>
   <si>
-    <t>C</t>
+    <t>B</t>
   </si>
   <si>
     <t>Operator</t>
@@ -100,28 +100,22 @@
     <t>Actual Weight (Kg)</t>
   </si>
   <si>
-    <t>CB</t>
-  </si>
-  <si>
-    <t>CB101</t>
-  </si>
-  <si>
     <t>POLY</t>
   </si>
   <si>
-    <t>CBM1312</t>
-  </si>
-  <si>
-    <t>FG023</t>
-  </si>
-  <si>
-    <t>OIL1</t>
-  </si>
-  <si>
-    <t>OIL45</t>
-  </si>
-  <si>
-    <t>STEA1</t>
+    <t>MAT005</t>
+  </si>
+  <si>
+    <t>MAT006</t>
+  </si>
+  <si>
+    <t>MAT007</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>MAT008</t>
   </si>
   <si>
     <t>-----&gt;&gt;</t>
@@ -184,7 +178,7 @@
     <t>Ram Up &amp; Discharge Door Open</t>
   </si>
   <si>
-    <t>keeping</t>
+    <t>Keeping</t>
   </si>
   <si>
     <t>Close Discharge Door &amp; Open Feed Door</t>
@@ -218,7 +212,7 @@
       <b/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +232,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="f2e6d9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6F7FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -274,7 +273,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -616,7 +615,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N26"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
@@ -694,7 +693,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>45967.87869212963</v>
+        <v>45967.93761574074</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -715,7 +714,7 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K4" s="3">
         <v>28</v>
@@ -755,28 +754,28 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B6" s="3">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C6" s="3">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
-        <v>159.1</v>
+        <v>158.3</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>22</v>
@@ -855,13 +854,13 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3">
-        <v>49.85</v>
+        <v>3.05</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -871,21 +870,21 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3">
-        <v>199.5</v>
+        <v>2.1</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -895,21 +894,21 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3">
-        <v>5</v>
+        <v>1.2</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3">
-        <v>5.1</v>
+        <v>1.18</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -919,21 +918,21 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3">
-        <v>100</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3">
-        <v>101.2</v>
+        <v>0.48</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -943,140 +942,160 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3">
-        <v>3</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3">
-        <v>3.05</v>
-      </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6">
+        <v>6.7</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
+        <v>6.8100000000000005</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6">
-        <v>358</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6">
-        <v>358.7</v>
-      </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="C16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" s="7"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="E17" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="G17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="I17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="K17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L17" s="7"/>
+      <c r="L17" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="M17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="7" t="s">
+      <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>49</v>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>13</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>69.4</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>83</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="3">
+        <v>14</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1090,34 +1109,34 @@
         <v>0</v>
       </c>
       <c r="D19" s="3">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="E19" s="3">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F19" s="3">
-        <v>69.4</v>
+        <v>130.1</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
       </c>
       <c r="H19" s="3">
-        <v>83</v>
+        <v>973</v>
       </c>
       <c r="I19" s="3">
-        <v>0</v>
+        <v>12.2</v>
       </c>
       <c r="J19" s="3">
-        <v>0.5</v>
+        <v>11.2</v>
       </c>
       <c r="K19" s="3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L19" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="M19" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N19" s="3">
         <v>55</v>
@@ -1128,40 +1147,40 @@
         <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E20" s="3">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F20" s="3">
-        <v>130.1</v>
+        <v>130.7</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
       </c>
       <c r="H20" s="3">
-        <v>973</v>
+        <v>148</v>
       </c>
       <c r="I20" s="3">
-        <v>12.2</v>
+        <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>11.2</v>
+        <v>11.8</v>
       </c>
       <c r="K20" s="3">
         <v>0</v>
       </c>
       <c r="L20" s="3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M20" s="3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="N20" s="3">
         <v>55</v>
@@ -1169,46 +1188,46 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3">
-        <v>130.7</v>
+        <v>113.6</v>
       </c>
       <c r="G21" s="3">
         <v>0</v>
       </c>
       <c r="H21" s="3">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="I21" s="3">
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>11.8</v>
+        <v>12.2</v>
       </c>
       <c r="K21" s="3">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L21" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M21" s="3">
         <v>0</v>
       </c>
       <c r="N21" s="3">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1216,37 +1235,37 @@
         <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
       </c>
       <c r="D22" s="3">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <v>113.6</v>
+        <v>138.1</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>
       </c>
       <c r="H22" s="3">
-        <v>77</v>
+        <v>826</v>
       </c>
       <c r="I22" s="3">
-        <v>0</v>
+        <v>15.7</v>
       </c>
       <c r="J22" s="3">
-        <v>12.2</v>
+        <v>14.8</v>
       </c>
       <c r="K22" s="3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L22" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="M22" s="3">
         <v>0</v>
@@ -1257,40 +1276,40 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
       </c>
       <c r="D23" s="3">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
       </c>
       <c r="F23" s="3">
-        <v>138.1</v>
+        <v>138.7</v>
       </c>
       <c r="G23" s="3">
         <v>0</v>
       </c>
       <c r="H23" s="3">
-        <v>826</v>
+        <v>234</v>
       </c>
       <c r="I23" s="3">
-        <v>15.7</v>
+        <v>0</v>
       </c>
       <c r="J23" s="3">
-        <v>14.8</v>
+        <v>15.5</v>
       </c>
       <c r="K23" s="3">
         <v>0</v>
       </c>
       <c r="L23" s="3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="M23" s="3">
         <v>0</v>
@@ -1301,7 +1320,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>51</v>
@@ -1310,107 +1329,107 @@
         <v>0</v>
       </c>
       <c r="D24" s="3">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F24" s="3">
-        <v>138.7</v>
+        <v>157</v>
       </c>
       <c r="G24" s="3">
         <v>0</v>
       </c>
       <c r="H24" s="3">
-        <v>234</v>
+        <v>759</v>
       </c>
       <c r="I24" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J24" s="3">
-        <v>15.5</v>
+        <v>18.5</v>
       </c>
       <c r="K24" s="3">
         <v>0</v>
       </c>
       <c r="L24" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M24" s="3">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="N24" s="3">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3">
+        <v>117</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>148.1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>16</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>19</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3">
+        <v>5</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+      <c r="N25" s="3">
         <v>53</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>113</v>
-      </c>
-      <c r="E25" s="3">
-        <v>150</v>
-      </c>
-      <c r="F25" s="3">
-        <v>157</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
-        <v>759</v>
-      </c>
-      <c r="I25" s="3">
-        <v>20</v>
-      </c>
-      <c r="J25" s="3">
-        <v>18.5</v>
-      </c>
-      <c r="K25" s="3">
-        <v>0</v>
-      </c>
-      <c r="L25" s="3">
-        <v>12</v>
-      </c>
-      <c r="M25" s="3">
-        <v>55</v>
-      </c>
-      <c r="N25" s="3">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D26" s="3">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
       </c>
       <c r="F26" s="3">
-        <v>148.1</v>
+        <v>125.5</v>
       </c>
       <c r="G26" s="3">
         <v>0</v>
       </c>
       <c r="H26" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I26" s="3">
         <v>0</v>
@@ -1422,61 +1441,17 @@
         <v>0</v>
       </c>
       <c r="L26" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M26" s="3">
         <v>0</v>
       </c>
       <c r="N26" s="3">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
-        <v>124</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3">
-        <v>125.5</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
-        <v>20</v>
-      </c>
-      <c r="I27" s="3">
-        <v>0</v>
-      </c>
-      <c r="J27" s="3">
-        <v>19</v>
-      </c>
-      <c r="K27" s="3">
-        <v>0</v>
-      </c>
-      <c r="L27" s="3">
-        <v>0</v>
-      </c>
-      <c r="M27" s="3">
-        <v>0</v>
-      </c>
-      <c r="N27" s="3">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="43">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="C3:E3"/>
@@ -1511,18 +1486,15 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="I14:N14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="I15:N15"/>
-    <mergeCell ref="A16:N16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>